<commit_message>
updated NF calcs with MAX2031 mixer and additional gain
</commit_message>
<xml_diff>
--- a/hardware/Graviton NF Calc 20160913.xlsx
+++ b/hardware/Graviton NF Calc 20160913.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="17985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="17985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MAX2031-1LNA" sheetId="3" r:id="rId2"/>
+    <sheet name="MAX2031-2LNA" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="35">
   <si>
     <t>Stage</t>
   </si>
@@ -126,6 +128,9 @@
   </si>
   <si>
     <t>Reflectionless LPF</t>
+  </si>
+  <si>
+    <t>MAX2031</t>
   </si>
 </sst>
 </file>
@@ -133,8 +138,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -194,8 +199,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,19 +541,19 @@
         <v>0.27</v>
       </c>
       <c r="E2" s="4">
-        <f>EXP(D2/10)</f>
-        <v>1.0273678027634894</v>
+        <f>10^(D2/10)</f>
+        <v>1.0641430182243161</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
       </c>
       <c r="G2" s="5">
-        <f>EXP(F2/10)</f>
+        <f>10^(F2/10)</f>
         <v>1</v>
       </c>
       <c r="H2" s="6">
         <f>E2</f>
-        <v>1.0273678027634894</v>
+        <v>1.0641430182243161</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>7</v>
@@ -568,20 +573,20 @@
         <v>1.5</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E11" si="0">EXP(D3/10)</f>
-        <v>1.1618342427282831</v>
+        <f t="shared" ref="E3:E11" si="0">10^(D3/10)</f>
+        <v>1.4125375446227544</v>
       </c>
       <c r="F3" s="4">
         <f>SUM(C2)</f>
         <v>18.399999999999999</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G11" si="1">EXP(F3/10)</f>
-        <v>6.2965382610266563</v>
+        <f t="shared" ref="G3:G11" si="1">10^(F3/10)</f>
+        <v>69.183097091893657</v>
       </c>
       <c r="H3" s="6">
         <f>H2+(E3-1)/G3</f>
-        <v>1.0530699006495579</v>
+        <v>1.070105999963552</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>
@@ -598,11 +603,11 @@
         <v>-2</v>
       </c>
       <c r="D4">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>0.81873075307798182</v>
+        <v>1.5848931924611136</v>
       </c>
       <c r="F4" s="4">
         <f>SUM(C2:C3)</f>
@@ -610,11 +615,11 @@
       </c>
       <c r="G4" s="5">
         <f t="shared" si="1"/>
-        <v>5.4194807051312059</v>
+        <v>48.977881936844632</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" ref="H4:H10" si="2">H3+(E4-1)/G4</f>
-        <v>1.0196221854929395</v>
+        <v>1.0820479862098196</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
@@ -635,7 +640,7 @@
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>2.585709659315846</v>
+        <v>8.9125093813374576</v>
       </c>
       <c r="F5" s="4">
         <f>SUM(C2:C4)</f>
@@ -643,11 +648,11 @@
       </c>
       <c r="G5" s="5">
         <f t="shared" si="1"/>
-        <v>4.4370955190036634</v>
+        <v>30.902954325135905</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="2"/>
-        <v>1.3769977823274906</v>
+        <v>1.3380917708295175</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -664,11 +669,11 @@
         <v>-1.4</v>
       </c>
       <c r="D6">
-        <v>-1.4</v>
+        <v>1.4</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0.86935823539880586</v>
+        <v>1.3803842646028848</v>
       </c>
       <c r="F6" s="4">
         <f>SUM(C2:C5)</f>
@@ -676,11 +681,11 @@
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>12.061276120444715</v>
+        <v>309.02954325135909</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="2"/>
-        <v>1.3661662779910839</v>
+        <v>1.3393226701817309</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>17</v>
@@ -701,7 +706,7 @@
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1.1618342427282831</v>
+        <v>1.4125375446227544</v>
       </c>
       <c r="F7" s="4">
         <f>SUM(C2:C6)</f>
@@ -709,11 +714,11 @@
       </c>
       <c r="G7" s="5">
         <f t="shared" si="1"/>
-        <v>10.485569724727576</v>
+        <v>223.87211385683412</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="2"/>
-        <v>1.3816002741378681</v>
+        <v>1.3411654077050232</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>8</v>
@@ -734,7 +739,7 @@
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2.1597662537849152</v>
+        <v>5.8884365535558905</v>
       </c>
       <c r="F8" s="4">
         <f>SUM(C2:C7)</f>
@@ -742,11 +747,11 @@
       </c>
       <c r="G8" s="5">
         <f t="shared" si="1"/>
-        <v>9.025013499434122</v>
+        <v>158.48931924611153</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="2"/>
-        <v>1.5101060380192888</v>
+        <v>1.3720093571699385</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>22</v>
@@ -763,11 +768,11 @@
         <v>-2</v>
       </c>
       <c r="D9">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0.81873075307798182</v>
+        <v>1.5848931924611136</v>
       </c>
       <c r="F9" s="4">
         <f>SUM(C2:C8)</f>
@@ -775,11 +780,11 @@
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>29.964100047397011</v>
+        <v>2511.8864315095811</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="2"/>
-        <v>1.5040564905062552</v>
+        <v>1.3722422073438652</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -797,7 +802,7 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>2.1597662537849152</v>
+        <v>5.8884365535558905</v>
       </c>
       <c r="F10" s="4">
         <f>SUM(C2:C9)</f>
@@ -805,11 +810,11 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>24.532530197109352</v>
+        <v>1584.8931924611156</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="2"/>
-        <v>1.5513311191102617</v>
+        <v>1.3753266022903567</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>22</v>
@@ -830,7 +835,7 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.3498588075760032</v>
+        <v>1.9952623149688797</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(C2:C10)</f>
@@ -838,11 +843,11 @@
       </c>
       <c r="G11" s="5">
         <f t="shared" si="1"/>
-        <v>33.115451958692312</v>
+        <v>3162.2776601683804</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" ref="H11" si="3">H10+(E11-1)/G11</f>
-        <v>1.5618959396663095</v>
+        <v>1.3756413318688201</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>32</v>
@@ -858,13 +863,13 @@
       </c>
       <c r="H12" s="2">
         <f>H11</f>
-        <v>1.5618959396663095</v>
+        <v>1.3756413318688201</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H13" s="2">
         <f>10*LOG(H12)</f>
-        <v>1.936520959086661</v>
+        <v>1.3850521595260088</v>
       </c>
       <c r="I13" t="s">
         <v>29</v>
@@ -884,4 +889,857 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.27</v>
+      </c>
+      <c r="E2" s="4">
+        <f>10^(D2/10)</f>
+        <v>1.0641430182243161</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <f>10^(F2/10)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <f>E2</f>
+        <v>1.0641430182243161</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>-1.5</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E11" si="0">10^(D3/10)</f>
+        <v>1.4125375446227544</v>
+      </c>
+      <c r="F3" s="4">
+        <f>SUM(C2)</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G11" si="1">10^(F3/10)</f>
+        <v>69.183097091893657</v>
+      </c>
+      <c r="H3" s="6">
+        <f>H2+(E3-1)/G3</f>
+        <v>1.070105999963552</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>-2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5848931924611136</v>
+      </c>
+      <c r="F4" s="4">
+        <f>SUM(C2:C3)</f>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>48.977881936844632</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H11" si="2">H3+(E4-1)/G4</f>
+        <v>1.0820479862098196</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>-7</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="F5" s="4">
+        <f>SUM(C2:C4)</f>
+        <v>14.899999999999999</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="1"/>
+        <v>30.902954325135905</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2118696302527496</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>-1.4</v>
+      </c>
+      <c r="D6">
+        <v>1.4</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3803842646028848</v>
+      </c>
+      <c r="F6" s="4">
+        <f>SUM(C2:C5)</f>
+        <v>7.8999999999999986</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>6.1659500186148204</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2735607343736906</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>-1.5</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4125375446227544</v>
+      </c>
+      <c r="F7" s="4">
+        <f>SUM(C2:C6)</f>
+        <v>6.4999999999999982</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>4.46683592150963</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3659163865336945</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>7.7</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>5.8884365535558905</v>
+      </c>
+      <c r="F8" s="4">
+        <f>SUM(C2:C7)</f>
+        <v>4.9999999999999982</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>3.1622776601683782</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="2"/>
+        <v>2.9117757571797247</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>-2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5848931924611136</v>
+      </c>
+      <c r="F9" s="4">
+        <f>SUM(C2:C8)</f>
+        <v>17</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>50.118723362727238</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="2"/>
+        <v>2.9234459106317199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>7.7</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.8884365535558905</v>
+      </c>
+      <c r="F10" s="4">
+        <f>SUM(C2:C9)</f>
+        <v>15</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>31.622776601683803</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0780318476963227</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9952623149688797</v>
+      </c>
+      <c r="F11" s="4">
+        <f>SUM(C2:C10)</f>
+        <v>27</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
+        <v>501.18723362727269</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0800176570868887</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C2:C11)</f>
+        <v>27</v>
+      </c>
+      <c r="H17" s="2">
+        <f>H11</f>
+        <v>3.0800176570868887</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="2">
+        <f>10*LOG(H17)</f>
+        <v>4.8855320622558116</v>
+      </c>
+      <c r="I18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="I11" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.27</v>
+      </c>
+      <c r="E2" s="4">
+        <f>10^(D2/10)</f>
+        <v>1.0641430182243161</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <f>10^(F2/10)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <f>E2</f>
+        <v>1.0641430182243161</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>-1.5</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E12" si="0">10^(D3/10)</f>
+        <v>1.4125375446227544</v>
+      </c>
+      <c r="F3" s="4">
+        <f>SUM(C2)</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G12" si="1">10^(F3/10)</f>
+        <v>69.183097091893657</v>
+      </c>
+      <c r="H3" s="6">
+        <f>H2+(E3-1)/G3</f>
+        <v>1.070105999963552</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.27</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0641430182243161</v>
+      </c>
+      <c r="F4" s="4">
+        <f>SUM(C2:C3)</f>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>48.977881936844632</v>
+      </c>
+      <c r="H4" s="6">
+        <f>H3+(E4-1)/G4</f>
+        <v>1.0714156323054942</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>-2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5848931924611136</v>
+      </c>
+      <c r="F5" s="4">
+        <f>SUM(C2:C4)</f>
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="1"/>
+        <v>3388.4415613920255</v>
+      </c>
+      <c r="H5" s="6">
+        <f>H3+(E5-1)/G5</f>
+        <v>1.0702786141821725</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>-7</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="F6" s="4">
+        <f>SUM(C2:C5)</f>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>2137.9620895022326</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" ref="H6:H12" si="2">H5+(E6-1)/G6</f>
+        <v>1.0721551078562053</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>-1.4</v>
+      </c>
+      <c r="D7">
+        <v>1.4</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3803842646028848</v>
+      </c>
+      <c r="F7" s="4">
+        <f>SUM(C2:C6)</f>
+        <v>26.299999999999997</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>426.57951880159294</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0730468156101816</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>-1.5</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4125375446227544</v>
+      </c>
+      <c r="F8" s="4">
+        <f>SUM(C2:C7)</f>
+        <v>24.9</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>309.02954325135909</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0743817609370341</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>7.7</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>5.8884365535558905</v>
+      </c>
+      <c r="F9" s="4">
+        <f>SUM(C2:C8)</f>
+        <v>23.4</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>218.77616239495524</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0967262270801545</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>-2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5848931924611136</v>
+      </c>
+      <c r="F10" s="4">
+        <f>SUM(C2:C9)</f>
+        <v>35.4</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>3467.3685045253224</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0968949121194567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>7.7</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>5.8884365535558905</v>
+      </c>
+      <c r="F11" s="4">
+        <f>SUM(C2:C10)</f>
+        <v>33.4</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
+        <v>2187.7616239495528</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0991293587337687</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9952623149688797</v>
+      </c>
+      <c r="F12" s="4">
+        <f>SUM(C2:C11)</f>
+        <v>45.4</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
+        <v>34673.685045253202</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0991580624124713</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C2:C12)</f>
+        <v>45.4</v>
+      </c>
+      <c r="H18" s="2">
+        <f>H12</f>
+        <v>1.0991580624124713</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="2">
+        <f>10*LOG(H18)</f>
+        <v>0.4106014983710855</v>
+      </c>
+      <c r="I19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I5" r:id="rId3"/>
+    <hyperlink ref="I6" r:id="rId4"/>
+    <hyperlink ref="I7" r:id="rId5"/>
+    <hyperlink ref="I8" r:id="rId6"/>
+    <hyperlink ref="I9" r:id="rId7"/>
+    <hyperlink ref="I11" r:id="rId8"/>
+    <hyperlink ref="I12" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>